<commit_message>
update mypy, pyright, standard libs ...
</commit_message>
<xml_diff>
--- a/_hunspell/de-DE/PreCheck_de-DE.xlsx
+++ b/_hunspell/de-DE/PreCheck_de-DE.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="12255" yWindow="1695" windowWidth="25170" windowHeight="14985"/>
+    <workbookView xWindow="12255" yWindow="1695" windowWidth="25170" windowHeight="14985" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Abkürzungen" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="824" uniqueCount="796">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="822" uniqueCount="796">
   <si>
     <t>Anmerkung</t>
   </si>
@@ -3037,7 +3037,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -3047,7 +3047,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B260"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="B16" sqref="B16"/>
     </sheetView>
@@ -4969,11 +4969,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B37"/>
+  <dimension ref="A1:B36"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B28" sqref="B28"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5025,238 +5025,230 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>633</v>
+        <v>634</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>656</v>
+        <v>659</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>634</v>
+        <v>635</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>659</v>
+        <v>660</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>635</v>
+        <v>707</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>660</v>
+        <v>708</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>707</v>
+        <v>636</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>708</v>
+        <v>661</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>636</v>
+        <v>647</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>661</v>
+        <v>670</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>647</v>
+        <v>637</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>670</v>
+        <v>671</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>637</v>
+        <v>645</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>671</v>
+        <v>678</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>645</v>
+        <v>638</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>678</v>
+        <v>672</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>638</v>
+        <v>639</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>672</v>
+        <v>679</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>639</v>
+        <v>655</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>679</v>
+        <v>666</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>655</v>
+        <v>709</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>666</v>
+        <v>710</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>709</v>
+        <v>646</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>710</v>
+        <v>663</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>646</v>
-      </c>
-      <c r="B19" s="4" t="s">
-        <v>663</v>
+        <v>685</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>685</v>
+        <v>648</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>662</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>648</v>
+        <v>641</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>662</v>
+        <v>675</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>641</v>
+        <v>650</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>675</v>
+        <v>680</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>650</v>
+        <v>654</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>680</v>
+        <v>673</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>654</v>
+        <v>642</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>673</v>
+        <v>665</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>642</v>
+        <v>643</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>665</v>
+        <v>676</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>643</v>
+        <v>763</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>676</v>
+        <v>764</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>763</v>
+        <v>651</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>764</v>
+        <v>667</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>651</v>
+        <v>649</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>667</v>
+        <v>674</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>649</v>
+        <v>653</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>674</v>
+        <v>677</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>677</v>
+        <v>668</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>652</v>
+        <v>644</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>668</v>
+        <v>664</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>644</v>
+        <v>711</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>664</v>
+        <v>712</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>711</v>
+        <v>748</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>712</v>
+        <v>749</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A34" s="1" t="s">
-        <v>748</v>
-      </c>
-      <c r="B34" s="4" t="s">
-        <v>749</v>
-      </c>
+      <c r="A34" s="1"/>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A35" s="1"/>
+      <c r="A35" s="1" t="s">
+        <v>435</v>
+      </c>
+      <c r="B35" s="4" t="s">
+        <v>494</v>
+      </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A36" s="1" t="s">
-        <v>435</v>
-      </c>
-      <c r="B36" s="4" t="s">
-        <v>494</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A37" s="1"/>
+      <c r="A36" s="1"/>
     </row>
   </sheetData>
   <sortState ref="A3:B32">

</xml_diff>